<commit_message>
All the TestCases have been updated with extent reports
</commit_message>
<xml_diff>
--- a/RestSharpNunitTestFramework/NunitRestSharpTestFramework/TestCaseConfiguration/TestCaseConfiguration.xlsx
+++ b/RestSharpNunitTestFramework/NunitRestSharpTestFramework/TestCaseConfiguration/TestCaseConfiguration.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="20">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -45,13 +45,37 @@
     <t>PROD</t>
   </si>
   <si>
-    <t>TestMethod1</t>
-  </si>
-  <si>
-    <t>TestMethod2</t>
-  </si>
-  <si>
-    <t>http://facebook.com/</t>
+    <t>http://jsonplaceholder.typicode.com/</t>
+  </si>
+  <si>
+    <t>validatingCommentsOfAParticularID</t>
+  </si>
+  <si>
+    <t>ValidatingCommentWithPostID</t>
+  </si>
+  <si>
+    <t>responseStatusCodeVerificationForTodos</t>
+  </si>
+  <si>
+    <t>responseStatusCodeVerificationForPhotos</t>
+  </si>
+  <si>
+    <t>responseStatusCodeVerificationForAlbums</t>
+  </si>
+  <si>
+    <t>responseStatusCodeVerificationForPosts</t>
+  </si>
+  <si>
+    <t>responseStatusCodeVerificationForComments</t>
+  </si>
+  <si>
+    <t>urlValidationOfaPhoto</t>
+  </si>
+  <si>
+    <t>urlValidationOfaPhotoParameterized</t>
+  </si>
+  <si>
+    <t>verifyPostedResource</t>
   </si>
 </sst>
 </file>
@@ -401,15 +425,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="43.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="37.140625" customWidth="1"/>
   </cols>
@@ -430,7 +454,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
@@ -439,23 +463,147 @@
         <v>6</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1"/>
+    <hyperlink ref="D3" r:id="rId2"/>
+    <hyperlink ref="D4" r:id="rId3"/>
+    <hyperlink ref="D6" r:id="rId4"/>
+    <hyperlink ref="D8" r:id="rId5"/>
+    <hyperlink ref="D5" r:id="rId6"/>
+    <hyperlink ref="D7" r:id="rId7"/>
+    <hyperlink ref="D9" r:id="rId8"/>
+    <hyperlink ref="D10" r:id="rId9"/>
+    <hyperlink ref="D11" r:id="rId10"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>